<commit_message>
Update horarios Excel files
</commit_message>
<xml_diff>
--- a/static/horarios/1-2024-v7.xlsx
+++ b/static/horarios/1-2024-v7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\schedule\static\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4B8CAC-13F1-4EAA-AE8B-D33F1332265F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69AC40B-6C88-4EC9-9781-135E60EEF501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
     <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'PROGRAMACIÓN I 2024'!$A$2:$DA$378</definedName>
     <definedName name="SegmentaciónDeDatos_13_14L">#N/A</definedName>
     <definedName name="SegmentaciónDeDatos_19_20L">#N/A</definedName>
@@ -25,8 +25,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -34,8 +34,8 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{841E416B-1EF1-43b6-AB56-02D37102CBD5}">
       <x15:pivotCaches>
-        <pivotCache cacheId="2" r:id="rId5"/>
-        <pivotCache cacheId="3" r:id="rId6"/>
+        <pivotCache cacheId="6" r:id="rId5"/>
+        <pivotCache cacheId="7" r:id="rId6"/>
       </x15:pivotCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{983426D0-5260-488c-9760-48F4B6AC55F4}">
@@ -104,7 +104,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="PROGRAMACIONES_PARCIALES" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1728,7 +1728,14 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1752,14 +1759,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2597,7 +2597,7 @@
   <c:extLst>
     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{723BEF56-08C2-4564-9609-F4CBC75E7E54}">
       <c15:pivotSource>
-        <c15:name>[1-2024.xlsx]PivotChartTable1</c15:name>
+        <c15:name>[1-2024-v7.xlsx]PivotChartTable1</c15:name>
         <c15:fmtId val="0"/>
       </c15:pivotSource>
       <c15:pivotOptions>
@@ -5205,7 +5205,7 @@
   <c:extLst>
     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{723BEF56-08C2-4564-9609-F4CBC75E7E54}">
       <c15:pivotSource>
-        <c15:name>[1-2024.xlsx]PivotChartTable2</c15:name>
+        <c15:name>[1-2024-v7.xlsx]PivotChartTable2</c15:name>
         <c15:fmtId val="0"/>
       </c15:pivotSource>
       <c15:pivotOptions>
@@ -7583,7 +7583,894 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1864DD7E-914F-4129-81BE-DE6895877F42}" name="PivotChartTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C494C86E-4DC1-488C-A314-1E315242265A}" name="PivotChartTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A1:B80" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="descending" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="78">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="79">
+    <i>
+      <x v="62"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="69"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="63"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="71"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="75"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="67"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="65"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="68"/>
+    </i>
+    <i>
+      <x v="76"/>
+    </i>
+    <i>
+      <x v="70"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="73"/>
+    </i>
+    <i>
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="66"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="72"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="77"/>
+    </i>
+    <i>
+      <x v="74"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="64"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de HORAS SEMANAL" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotHierarchies count="111">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="13"/>
+  </rowHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{44433962-1CF7-4059-B4EE-95C3D5FFCF73}">
+      <x15:pivotTableData rowCount="79" columnCount="1" cacheId="531005254">
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>38</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>38</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>36</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>36</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>36</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>34</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>34</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>32</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>32</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>31</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>30</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>28</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>26</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>25</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>24</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>23</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>23</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>22</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>22</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>22</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>22</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>20</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>20</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>20</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>20</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>18</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>18</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>14</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>12</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>10</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>2044</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+      </x15:pivotTableData>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsx!PROGRAMACIONES_PARCIALES">
+        <x15:activeTabTopLevelEntity name="[PROGRAMACIONES_PARCIALES]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1864DD7E-914F-4129-81BE-DE6895877F42}" name="PivotChartTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:I19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -8380,895 +9267,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C494C86E-4DC1-488C-A314-1E315242265A}" name="PivotChartTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A1:B80" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="descending" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="78">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item x="52"/>
-        <item x="53"/>
-        <item x="54"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="57"/>
-        <item x="58"/>
-        <item x="59"/>
-        <item x="60"/>
-        <item x="61"/>
-        <item x="62"/>
-        <item x="63"/>
-        <item x="64"/>
-        <item x="65"/>
-        <item x="66"/>
-        <item x="67"/>
-        <item x="68"/>
-        <item x="69"/>
-        <item x="70"/>
-        <item x="71"/>
-        <item x="72"/>
-        <item x="73"/>
-        <item x="74"/>
-        <item x="75"/>
-        <item x="76"/>
-        <item x="77"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="79">
-    <i>
-      <x v="62"/>
-    </i>
-    <i>
-      <x v="49"/>
-    </i>
-    <i>
-      <x v="69"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="53"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="56"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="63"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="71"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="75"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="55"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="67"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="54"/>
-    </i>
-    <i>
-      <x v="65"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="68"/>
-    </i>
-    <i>
-      <x v="76"/>
-    </i>
-    <i>
-      <x v="70"/>
-    </i>
-    <i>
-      <x v="57"/>
-    </i>
-    <i>
-      <x v="73"/>
-    </i>
-    <i>
-      <x v="61"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="66"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="72"/>
-    </i>
-    <i>
-      <x v="59"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="60"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="58"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="77"/>
-    </i>
-    <i>
-      <x v="74"/>
-    </i>
-    <i>
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="64"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Suma de HORAS SEMANAL" fld="1" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotHierarchies count="111">
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-  </pivotHierarchies>
-  <rowHierarchiesUsage count="1">
-    <rowHierarchyUsage hierarchyUsage="13"/>
-  </rowHierarchiesUsage>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{44433962-1CF7-4059-B4EE-95C3D5FFCF73}">
-      <x15:pivotTableData rowCount="79" columnCount="1" cacheId="531005254">
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>38</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>38</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>36</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>36</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>36</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>34</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>34</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>32</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>32</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>31</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>30</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>26</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>25</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>24</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>23</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>23</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>22</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>22</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>22</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>22</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>20</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>20</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>20</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>20</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>18</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>18</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>14</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>12</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>10</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>2044</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-      </x15:pivotTableData>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
-      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsx!PROGRAMACIONES_PARCIALES">
-        <x15:activeTabTopLevelEntity name="[PROGRAMACIONES_PARCIALES]"/>
-      </x15:pivotTableUISettings>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E51D2C13-18A8-44E4-9514-17D00C659F63}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E51D2C13-18A8-44E4-9514-17D00C659F63}" name="TablaDinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B82" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -9737,7 +9737,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3EA41CB7-E3A8-430F-B4AE-F3DE60532250}" name="TablaDinámica3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3EA41CB7-E3A8-430F-B4AE-F3DE60532250}" name="TablaDinámica3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D30:E47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -10136,21 +10136,21 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{078F9945-76D9-4C04-BF83-65B682ED43CC}" name="PROGRAMACIONES_PARCIALES" displayName="PROGRAMACIONES_PARCIALES" ref="A2:DI379" tableType="queryTable" totalsRowCount="1">
   <autoFilter ref="A2:DI378" xr:uid="{078F9945-76D9-4C04-BF83-65B682ED43CC}"/>
   <tableColumns count="113">
-    <tableColumn id="105" xr3:uid="{87D8DA09-394D-4852-A9F6-06583A29B0FC}" uniqueName="105" name="Source.Name" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{61E6697F-673F-4B06-8904-614D56FA179F}" uniqueName="2" name="FICHA" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{3DE7CF3C-20A5-45C3-A939-9C88D01D0FE9}" uniqueName="3" name="FORMACIÓN" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{363CDC32-9FD0-4CEB-8D8D-B919E15FAA38}" uniqueName="4" name="TITULAR" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="105" xr3:uid="{87D8DA09-394D-4852-A9F6-06583A29B0FC}" uniqueName="105" name="Source.Name" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{61E6697F-673F-4B06-8904-614D56FA179F}" uniqueName="2" name="FICHA" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3DE7CF3C-20A5-45C3-A939-9C88D01D0FE9}" uniqueName="3" name="FORMACIÓN" queryTableFieldId="3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{363CDC32-9FD0-4CEB-8D8D-B919E15FAA38}" uniqueName="4" name="TITULAR" queryTableFieldId="4" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{8B226D1B-BFF2-49BB-B758-EE4B851E70DA}" uniqueName="5" name="TRIMESTRE_ACADÉMICO" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{78A28FE9-7887-4ACB-88EB-DFAD7F40A943}" uniqueName="6" name="COMPETENCIA" queryTableFieldId="6" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{BF62391A-F89A-44CC-A8B6-3E506A304062}" uniqueName="7" name="NOMBRE_COMPETENCIA" queryTableFieldId="7" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{78A28FE9-7887-4ACB-88EB-DFAD7F40A943}" uniqueName="6" name="COMPETENCIA" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{BF62391A-F89A-44CC-A8B6-3E506A304062}" uniqueName="7" name="NOMBRE_COMPETENCIA" queryTableFieldId="7" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{5C00E006-DEB8-4B45-B7E3-B775FAC56914}" uniqueName="8" name="RAP 1" queryTableFieldId="8"/>
     <tableColumn id="9" xr3:uid="{49EFD39C-728B-4C81-8193-D20CD8923D69}" uniqueName="9" name="RAP 2" queryTableFieldId="9"/>
     <tableColumn id="10" xr3:uid="{B6F8F457-5381-4426-9F22-D87B3BAE1E1B}" uniqueName="10" name="RAP 3" queryTableFieldId="10"/>
     <tableColumn id="11" xr3:uid="{0EECA1C3-E5FD-4979-BEEB-1A297BEFAD06}" uniqueName="11" name="RAP 4" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{D0A977BB-7A27-4EF0-B307-4BAD18A1D841}" uniqueName="12" name="RAP 5" queryTableFieldId="12"/>
     <tableColumn id="13" xr3:uid="{F8C8EBB1-C23A-49D5-B16B-0380006A1DDD}" uniqueName="13" name="RAP 6" queryTableFieldId="13"/>
-    <tableColumn id="14" xr3:uid="{E8FBDA0F-CDFB-4BBD-AF1C-B9773372BC4C}" uniqueName="14" name="INSTRUCTOR" queryTableFieldId="14" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{81F91995-5EA0-4D2A-9C41-99CFC65133C2}" uniqueName="15" name="NOMBRE DE LA COMPETENCIA 2" queryTableFieldId="15" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{E8FBDA0F-CDFB-4BBD-AF1C-B9773372BC4C}" uniqueName="14" name="INSTRUCTOR" queryTableFieldId="14" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{81F91995-5EA0-4D2A-9C41-99CFC65133C2}" uniqueName="15" name="NOMBRE DE LA COMPETENCIA 2" queryTableFieldId="15" dataDxfId="1"/>
     <tableColumn id="16" xr3:uid="{34761CDE-83A0-4FFA-B1E9-1FEBE9DC1075}" uniqueName="16" name="HORAS_SEMANAL" queryTableFieldId="16"/>
     <tableColumn id="17" xr3:uid="{B25F73F1-9F14-47B9-B123-7A878796CCA7}" uniqueName="17" name="HORAS POR TRIMESTRE" queryTableFieldId="17"/>
     <tableColumn id="18" xr3:uid="{3F05A4C2-F912-4CB3-AA16-A7656C50765A}" uniqueName="18" name="6-7L" totalsRowFunction="custom" queryTableFieldId="18">
@@ -10713,8 +10713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C46E5B-3CE7-4F67-9F7E-3BDF34AAB992}">
   <dimension ref="A1:DI379"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="DC1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:DI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10728,9 +10728,9 @@
     <col min="7" max="7" width="81.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="81.109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="81.109375" customWidth="1"/>
     <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="24" customWidth="1"/>
     <col min="18" max="20" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="22" max="33" width="8.88671875" bestFit="1" customWidth="1"/>
@@ -32859,7 +32859,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R379:DA379">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>